<commit_message>
Restore Point - extend test installer to show a custom screen in response to error from InitProps
</commit_message>
<xml_diff>
--- a/Documentation/AI RISA Installer Properties.xlsx
+++ b/Documentation/AI RISA Installer Properties.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Advanced Installer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6167BF-1B1F-40F3-B595-104B823E2B3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B3BAE9-C14E-4F8D-B7D8-33B92881F5CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24588" yWindow="6972" windowWidth="22332" windowHeight="15492" activeTab="1" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
+    <workbookView xWindow="-18600" yWindow="564" windowWidth="18024" windowHeight="17172" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Extended Properties" sheetId="5" r:id="rId1"/>
-    <sheet name="InitProperties CA" sheetId="6" r:id="rId2"/>
+    <sheet name="PropList-April2" sheetId="7" r:id="rId1"/>
+    <sheet name="InitProperties CA-Mar22" sheetId="6" r:id="rId2"/>
+    <sheet name="Extended Properties-Mar21" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="162">
   <si>
     <t>MSI required properties</t>
   </si>
@@ -451,13 +452,82 @@
   </si>
   <si>
     <t>Action.Success - in all other cases (except RISA_WARN_xxx) Action.Failure is returned</t>
+  </si>
+  <si>
+    <t>filled by InitProperties CA (xml serialized class), deserialized by RemoveInstalledProducts CA</t>
+  </si>
+  <si>
+    <t>new (Apr2)</t>
+  </si>
+  <si>
+    <t>tentative, subject to change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for possible use by dialogs and silent install </t>
+  </si>
+  <si>
+    <t>RISA_ERR_INSTALL_OLD_VERSION</t>
+  </si>
+  <si>
+    <t>Action.Failure</t>
+  </si>
+  <si>
+    <t>Action.Success</t>
+  </si>
+  <si>
+    <t>written to Session.Log()</t>
+  </si>
+  <si>
+    <t>flag - in silent install flag, may not be needed (tbd)</t>
+  </si>
+  <si>
+    <t>These properties will need to be added to the AIP</t>
+  </si>
+  <si>
+    <t>this list doesn't include the standard MSI properties you get without any effort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silent install file - likely to be dropped in favor of MSI props </t>
+  </si>
+  <si>
+    <t>prefer a 4 part version, but OK w 3</t>
+  </si>
+  <si>
+    <t>RISA_CA_TRACE</t>
+  </si>
+  <si>
+    <t>if empty, no trace file is written, if DESKTOP write a trace log to desktop; other values are presently ignored</t>
+  </si>
+  <si>
+    <t>Extended Properties</t>
+  </si>
+  <si>
+    <t>output values, most are set by the InitProperties CA; other uses by other CAs are noted below</t>
+  </si>
+  <si>
+    <t>when newer is already installed</t>
+  </si>
+  <si>
+    <t>meaning</t>
+  </si>
+  <si>
+    <t>if RISA_REGISTRY_PRODUCT_NAME is blank, InitProperties will set it to MSI ProductName</t>
+  </si>
+  <si>
+    <t>dropped (Apr2)</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>enh (Apr2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,8 +577,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFA861E9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFA861E9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFA861E9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -518,6 +632,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -558,6 +678,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,6 +694,7 @@
   <colors>
     <mruColors>
       <color rgb="FF00FF00"/>
+      <color rgb="FFA861E9"/>
     </mruColors>
   </colors>
   <extLst>
@@ -876,11 +1004,551 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3BD056-C256-4065-A1B5-A0BB5D81AAD8}">
+  <dimension ref="B2:M44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" style="1" customWidth="1"/>
+    <col min="3" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="11.44140625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="9.109375" style="1"/>
+    <col min="10" max="10" width="11.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="1"/>
+    <col min="12" max="12" width="21.109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G6" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G14" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="K23" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="M23" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M26" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M27" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M28" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G30" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M30" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H33" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="11"/>
+      <c r="C38" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="11"/>
+      <c r="C39" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="11"/>
+      <c r="C40" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41" s="11"/>
+      <c r="C41" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" s="13"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="13"/>
+      <c r="C44" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88275DA6-E210-4F4E-A4B1-5157A653E585}">
+  <dimension ref="B2:M30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G5" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G11" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="K21" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H24" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H25" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H26" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H27" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H30" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC0BC72-5B03-4290-9EED-883BE221AEC1}">
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1443,194 +2111,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88275DA6-E210-4F4E-A4B1-5157A653E585}">
-  <dimension ref="B2:M30"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.109375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G5" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G11" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C17" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="K21" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="M21" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="H22" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="H23" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="H24" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="H25" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="H26" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="H27" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C29" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="H30" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
C/U + impl optional RISA_CA_DEBUG prop, setting TRACEFILE via installer property r/t hardwired. Restore Point prior to extend InitProps to check for running RISA / ADAPT processes
</commit_message>
<xml_diff>
--- a/Documentation/AI RISA Installer Properties.xlsx
+++ b/Documentation/AI RISA Installer Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Advanced Installer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B3BAE9-C14E-4F8D-B7D8-33B92881F5CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EE8003-C6F3-43CF-8703-720334101320}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18600" yWindow="564" windowWidth="18024" windowHeight="17172" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
+    <workbookView xWindow="-30612" yWindow="804" windowWidth="18468" windowHeight="13992" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="PropList-April2" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="164">
   <si>
     <t>MSI required properties</t>
   </si>
@@ -521,6 +521,12 @@
   </si>
   <si>
     <t>enh (Apr2)</t>
+  </si>
+  <si>
+    <t>drop-&gt;</t>
+  </si>
+  <si>
+    <t>TODO identify every other place where Failure is returned</t>
   </si>
 </sst>
 </file>
@@ -637,7 +643,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FFA861E9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,8 +699,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFA861E9"/>
       <color rgb="FF00FF00"/>
-      <color rgb="FFA861E9"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1005,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3BD056-C256-4065-A1B5-A0BB5D81AAD8}">
-  <dimension ref="B2:M44"/>
+  <dimension ref="B2:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1123,7 +1129,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
         <v>55</v>
       </c>
@@ -1131,7 +1137,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
         <v>56</v>
       </c>
@@ -1139,7 +1145,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C19" s="1" t="s">
         <v>61</v>
       </c>
@@ -1147,7 +1153,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>99</v>
       </c>
@@ -1155,7 +1161,15 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L21" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
         <v>82</v>
       </c>
@@ -1163,7 +1177,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.3">
       <c r="K23" s="10" t="s">
         <v>157</v>
       </c>
@@ -1171,7 +1185,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.3">
       <c r="H24" s="1" t="s">
         <v>121</v>
       </c>
@@ -1182,7 +1196,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:15" x14ac:dyDescent="0.3">
       <c r="H25" s="1" t="s">
         <v>122</v>
       </c>
@@ -1193,7 +1207,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:15" x14ac:dyDescent="0.3">
       <c r="H26" s="1" t="s">
         <v>123</v>
       </c>
@@ -1201,7 +1215,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:15" x14ac:dyDescent="0.3">
       <c r="H27" s="1" t="s">
         <v>124</v>
       </c>
@@ -1209,7 +1223,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="G28" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="H28" s="1" t="s">
         <v>125</v>
       </c>
@@ -1217,7 +1234,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="G29" s="14" t="s">
+        <v>162</v>
+      </c>
       <c r="H29" s="1" t="s">
         <v>126</v>
       </c>
@@ -1228,7 +1248,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:15" x14ac:dyDescent="0.3">
       <c r="G30" s="2" t="s">
         <v>140</v>
       </c>
@@ -1242,7 +1262,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Docs complete for Loud Install CAs and usage
</commit_message>
<xml_diff>
--- a/Documentation/AI RISA Installer Properties.xlsx
+++ b/Documentation/AI RISA Installer Properties.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Advanced Installer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EE8003-C6F3-43CF-8703-720334101320}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9C0FC7-9DF0-49DC-AA7E-141B05C7B5E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30612" yWindow="804" windowWidth="18468" windowHeight="13992" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
+    <workbookView xWindow="3912" yWindow="2712" windowWidth="20916" windowHeight="17292" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
   </bookViews>
   <sheets>
-    <sheet name="PropList-April2" sheetId="7" r:id="rId1"/>
+    <sheet name="PropList-Apr9" sheetId="7" r:id="rId1"/>
     <sheet name="InitProperties CA-Mar22" sheetId="6" r:id="rId2"/>
     <sheet name="Extended Properties-Mar21" sheetId="5" r:id="rId3"/>
   </sheets>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="181">
   <si>
     <t>MSI required properties</t>
   </si>
@@ -454,12 +454,6 @@
     <t>Action.Success - in all other cases (except RISA_WARN_xxx) Action.Failure is returned</t>
   </si>
   <si>
-    <t>filled by InitProperties CA (xml serialized class), deserialized by RemoveInstalledProducts CA</t>
-  </si>
-  <si>
-    <t>new (Apr2)</t>
-  </si>
-  <si>
     <t>tentative, subject to change</t>
   </si>
   <si>
@@ -469,9 +463,6 @@
     <t>RISA_ERR_INSTALL_OLD_VERSION</t>
   </si>
   <si>
-    <t>Action.Failure</t>
-  </si>
-  <si>
     <t>Action.Success</t>
   </si>
   <si>
@@ -493,40 +484,100 @@
     <t>prefer a 4 part version, but OK w 3</t>
   </si>
   <si>
-    <t>RISA_CA_TRACE</t>
-  </si>
-  <si>
-    <t>if empty, no trace file is written, if DESKTOP write a trace log to desktop; other values are presently ignored</t>
-  </si>
-  <si>
     <t>Extended Properties</t>
   </si>
   <si>
     <t>output values, most are set by the InitProperties CA; other uses by other CAs are noted below</t>
   </si>
   <si>
-    <t>when newer is already installed</t>
-  </si>
-  <si>
     <t>meaning</t>
   </si>
   <si>
-    <t>if RISA_REGISTRY_PRODUCT_NAME is blank, InitProperties will set it to MSI ProductName</t>
-  </si>
-  <si>
-    <t>dropped (Apr2)</t>
-  </si>
-  <si>
-    <t>TODO</t>
-  </si>
-  <si>
-    <t>enh (Apr2)</t>
-  </si>
-  <si>
-    <t>drop-&gt;</t>
-  </si>
-  <si>
-    <t>TODO identify every other place where Failure is returned</t>
+    <t>optional property, currently only one value is implemented: TRACEFILE</t>
+  </si>
+  <si>
+    <t>InitProperties() and RemoveInstalledProducts() CAs write some basic info to this file, out of the box</t>
+  </si>
+  <si>
+    <t>to avoid AI's generic error handling</t>
+  </si>
+  <si>
+    <t>(giving no idea of what went wrong)</t>
+  </si>
+  <si>
+    <t>client should instead check RISA_STATUS_CODE</t>
+  </si>
+  <si>
+    <t>all CAs changed to always return Action.Success</t>
+  </si>
+  <si>
+    <t>RISA_CA_DEBUG (optional)</t>
+  </si>
+  <si>
+    <t>this can be extended to write more info as needed via calls within the CA to Trace()</t>
+  </si>
+  <si>
+    <t>this condition (3 part ProductVersion) now returns RISA_STS_OK</t>
+  </si>
+  <si>
+    <t>RISA_ERR_REMOVE_INSTALLED_PRODUCT</t>
+  </si>
+  <si>
+    <t>could not remove an installed product</t>
+  </si>
+  <si>
+    <t>RISA_ERR_PRODUCT_ACTIVE</t>
+  </si>
+  <si>
+    <t>RISA or ADAPT product(s) are active</t>
+  </si>
+  <si>
+    <t>new (Apr9)</t>
+  </si>
+  <si>
+    <t>revised (Apr9)</t>
+  </si>
+  <si>
+    <t>new status codes (Apr9)</t>
+  </si>
+  <si>
+    <t>dropped (Apr9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> used to transfer data from InitProperties() to RemoveInstalledProducts() CAs</t>
+  </si>
+  <si>
+    <t>&amp; optionally display RISA_STATUS_TEXT</t>
+  </si>
+  <si>
+    <t>not "Demo" or "Standalone"</t>
+  </si>
+  <si>
+    <t>unknown ProductName</t>
+  </si>
+  <si>
+    <t>ProductVersion not 3 or 4 parts</t>
+  </si>
+  <si>
+    <t>dropped unneeded status code (Apr9)</t>
+  </si>
+  <si>
+    <t>newer version is already installed</t>
+  </si>
+  <si>
+    <t>same as RISA_USERFILES, dropped, along with DetectRoaming CA</t>
+  </si>
+  <si>
+    <t>if present, and set to TRACEFILE, file "CustomAction_trace.txt" is output to the desktop</t>
+  </si>
+  <si>
+    <t>Legend:</t>
+  </si>
+  <si>
+    <t>Green = new or changed</t>
+  </si>
+  <si>
+    <t>Autumnal = dropped</t>
   </si>
 </sst>
 </file>
@@ -591,13 +642,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FFA861E9"/>
@@ -627,8 +671,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -638,12 +689,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA861E9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -690,7 +735,7 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,8 +744,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FFA861E9"/>
-      <color rgb="FF00FF00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1011,47 +1056,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3BD056-C256-4065-A1B5-A0BB5D81AAD8}">
-  <dimension ref="B2:O44"/>
+  <dimension ref="B2:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.88671875" style="1" customWidth="1"/>
-    <col min="3" max="6" width="9.109375" style="1"/>
-    <col min="7" max="7" width="11.44140625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="9.109375" style="1"/>
-    <col min="10" max="10" width="11.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1" customWidth="1"/>
+    <col min="4" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="6.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="1"/>
+    <col min="10" max="10" width="22.88671875" style="1" customWidth="1"/>
     <col min="11" max="11" width="9.109375" style="1"/>
-    <col min="12" max="12" width="21.109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="1"/>
+    <col min="12" max="12" width="24.109375" style="1" customWidth="1"/>
+    <col min="13" max="14" width="9.109375" style="1"/>
+    <col min="15" max="15" width="4.5546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="3.88671875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="G6" s="12" t="s">
+    <row r="6" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G6" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>58</v>
       </c>
@@ -1059,7 +1118,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>51</v>
       </c>
@@ -1067,7 +1126,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>108</v>
       </c>
@@ -1075,297 +1134,386 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="H10" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G11" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
-        <v>152</v>
-      </c>
+      <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="G14" s="12" t="s">
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G16" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="K25" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="H26" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="H27" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="H28" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q28" s="2"/>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="H29" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C20" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="L21" s="14" t="s">
+    <row r="30" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="H30" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="P30" s="2"/>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="D31" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="O31" s="2"/>
+      <c r="P31" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="F32" s="2"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="K32" s="5"/>
+      <c r="M32" s="5"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F33" s="2"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="2"/>
+      <c r="K33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D34" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F35" s="2"/>
+      <c r="H35" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F36" s="2"/>
+      <c r="H36" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="K23" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="M23" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="H24" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M24" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="H25" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M25" s="9" t="s">
+      <c r="K36" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H39" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B41" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B44" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C44" s="12"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B45" s="12"/>
+      <c r="C45" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B47" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B48" s="10"/>
+      <c r="C48" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="10"/>
+      <c r="C49" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="10"/>
+      <c r="C50" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="10"/>
+      <c r="C51" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="H26" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M26" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="H27" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M27" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M28" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="M29" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="G30" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="M30" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C32" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H33" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="11"/>
-      <c r="C38" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="11"/>
-      <c r="C39" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="11"/>
-      <c r="C40" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="11"/>
-      <c r="C41" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="C43" s="13"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="13"/>
-      <c r="C44" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="G44" s="13" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documentation for Silent Install
</commit_message>
<xml_diff>
--- a/Documentation/AI RISA Installer Properties.xlsx
+++ b/Documentation/AI RISA Installer Properties.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Advanced Installer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BD2376-B529-4CBA-A3A9-C7793B810D97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6247E12A-1E83-4965-BB54-C68B7AC2B4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25272" yWindow="5580" windowWidth="23748" windowHeight="17628" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
+    <workbookView xWindow="-27672" yWindow="4188" windowWidth="18888" windowHeight="17832" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
   </bookViews>
   <sheets>
-    <sheet name="PropList-Apr9" sheetId="7" r:id="rId1"/>
-    <sheet name="InitProperties CA-Mar22" sheetId="6" r:id="rId2"/>
-    <sheet name="Extended Properties-Mar21" sheetId="5" r:id="rId3"/>
+    <sheet name="PropList-Jun15" sheetId="8" r:id="rId1"/>
+    <sheet name="PropList-Apr9" sheetId="7" r:id="rId2"/>
+    <sheet name="InitProperties CA-Mar22" sheetId="6" r:id="rId3"/>
+    <sheet name="Extended Properties-Mar21" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="207">
   <si>
     <t>MSI required properties</t>
   </si>
@@ -593,6 +594,69 @@
   </si>
   <si>
     <t>For short-cuts whose text is property assigned, this is resolved at installer Build time, not Run time, and so this must be set by Tooling and Built.</t>
+  </si>
+  <si>
+    <t>CA returns a text code indicating what happened, one of:</t>
+  </si>
+  <si>
+    <t>all other values are ignored, resulting in no trace file</t>
+  </si>
+  <si>
+    <t>all Loud CAs always return Action.Success</t>
+  </si>
+  <si>
+    <t>(Loud) CA ActionResult return</t>
+  </si>
+  <si>
+    <t>contains more verbose details of RISA_STATUS_CODE - written to Session.Log()</t>
+  </si>
+  <si>
+    <t>Transfer properties - passing the result of one custom action to another</t>
+  </si>
+  <si>
+    <t>(Loud) CA output values, most are set by the InitProperties CA; other uses by other CAs are noted below</t>
+  </si>
+  <si>
+    <t>RISA_SI_PREINSTALL_RESULT</t>
+  </si>
+  <si>
+    <t>contents</t>
+  </si>
+  <si>
+    <t>the silent CA reads this status to determine whether to abort the installation (the exe cannot)</t>
+  </si>
+  <si>
+    <t>Properties assigned from dialogs or from silent install</t>
+  </si>
+  <si>
+    <t>RISA_CHECK_UPDATES</t>
+  </si>
+  <si>
+    <t>assigned to Region key in the registry for certain products</t>
+  </si>
+  <si>
+    <t>assigned to LocalUpdateCheck registry key</t>
+  </si>
+  <si>
+    <t>Properties useful for testing (assign from command line or in aip)</t>
+  </si>
+  <si>
+    <t>RISA_IS_ROAMING_PROFILE</t>
+  </si>
+  <si>
+    <t>returned by InitProps.assignDocumentPath(), used to control dialogs</t>
+  </si>
+  <si>
+    <t>APPDIR</t>
+  </si>
+  <si>
+    <t>standard AI property, directory where the application will be installed</t>
+  </si>
+  <si>
+    <t>int.ToString() value, returned  by Silent-PreInstall pre-req exe, read downstream by SilentInitProperties CA</t>
+  </si>
+  <si>
+    <t>serialized installed product info discovered in InitProperties() CA for potential removal by RemoveInstalledProducts() CA</t>
   </si>
 </sst>
 </file>
@@ -1070,11 +1134,396 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C1A5645-D1FB-4A1B-B8EC-0860F5606EBD}">
+  <dimension ref="B2:O52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" style="1" customWidth="1"/>
+    <col min="3" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="6.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="1"/>
+    <col min="10" max="10" width="22.88671875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="1"/>
+    <col min="12" max="12" width="24.109375" style="1" customWidth="1"/>
+    <col min="13" max="14" width="9.109375" style="1"/>
+    <col min="15" max="15" width="4.5546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="3.88671875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G6" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G14" s="11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="K23" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="H24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="H25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="H26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="H27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="H28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D29" s="2"/>
+      <c r="H29" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="F30" s="2"/>
+      <c r="H30" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="F31" s="2"/>
+      <c r="H31" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C34" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B37" s="8"/>
+      <c r="G37" s="11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="2"/>
+      <c r="C38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H40" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="8"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="10"/>
+      <c r="C44" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="10"/>
+      <c r="C45" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="10"/>
+      <c r="C46" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B48" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B50" s="2"/>
+      <c r="C50" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="H51" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I51" s="2"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I52" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3BD056-C256-4065-A1B5-A0BB5D81AAD8}">
   <dimension ref="B2:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1553,7 +2002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88275DA6-E210-4F4E-A4B1-5157A653E585}">
   <dimension ref="B2:M30"/>
   <sheetViews>
@@ -1743,7 +2192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC0BC72-5B03-4290-9EED-883BE221AEC1}">
   <dimension ref="A1:T54"/>
   <sheetViews>

</xml_diff>